<commit_message>
Add sample and change for color grouping
</commit_message>
<xml_diff>
--- a/Grocery Purchase Order.xlsx
+++ b/Grocery Purchase Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1stdesignglobal-my.sharepoint.com/personal/shipping_firstdesign_global/Documents/FDG-Shipping server/Ariel/Projects/Automate_Correct_Form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC1048FF81DF76705BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E962F5A-77F7-4EE2-889B-8BD0FD734F0F}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048FF81DF76705BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCAA5862-AC4E-49AE-811C-DDD5C4961CD8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>product name</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Durian</t>
   </si>
 </sst>
 </file>
@@ -106,6 +112,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,6 +428,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>60</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>